<commit_message>
r0 con traduccion de paises
</commit_message>
<xml_diff>
--- a/SIR_provincias/r0avanzadas.xlsx
+++ b/SIR_provincias/r0avanzadas.xlsx
@@ -1,21 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrador\Desktop\libros\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A06A6A-7259-4CCD-818D-F9D8CA833E7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9BA7A6C-7C17-4ED5-A19C-B1CC77E6A513}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E304EFAB-3164-4D20-84F7-4CCF7EACFDA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{E304EFAB-3164-4D20-84F7-4CCF7EACFDA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="52">
   <si>
     <t>R0_AUS_VA7D</t>
   </si>
@@ -110,6 +111,84 @@
   <si>
     <t>R0_USA_VA7D</t>
   </si>
+  <si>
+    <t>AUSTRIA</t>
+  </si>
+  <si>
+    <t>NELGICA</t>
+  </si>
+  <si>
+    <t>AUSTRALIA</t>
+  </si>
+  <si>
+    <t>BRAZIL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHILE </t>
+  </si>
+  <si>
+    <t xml:space="preserve">CHINA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REPUBLICA DOMINICANA </t>
+  </si>
+  <si>
+    <t>ESPAÑA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FRANCIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">REINO UNIDO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ISRAEL </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ITALIA </t>
+  </si>
+  <si>
+    <t>COREAL DEL SUR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MEXICO </t>
+  </si>
+  <si>
+    <t xml:space="preserve">NORUEGA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SINGAPUR </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUECIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ESTADOS UNIDOS </t>
+  </si>
+  <si>
+    <t>GUATEMALA</t>
+  </si>
+  <si>
+    <t>HONDURAS</t>
+  </si>
+  <si>
+    <t>PERU</t>
+  </si>
+  <si>
+    <t>PORTUGAL</t>
+  </si>
+  <si>
+    <t>EL SALVADOR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALEMANIA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">COSTA RICA </t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUIZA </t>
+  </si>
 </sst>
 </file>
 
@@ -165,7 +244,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -463,13 +542,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F5C751DA-1E2E-4BF5-88D8-F1E1A8C7CED0}">
   <dimension ref="A1:AA109"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:XFD1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -549,22 +628,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43852</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43853</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43854</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43855</v>
       </c>
@@ -575,7 +654,7 @@
         <v>6.1333333335389204</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43856</v>
       </c>
@@ -586,7 +665,7 @@
         <v>6.1333333333333302</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43857</v>
       </c>
@@ -600,7 +679,7 @@
         <v>3.7533333385127201</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43858</v>
       </c>
@@ -614,7 +693,7 @@
         <v>4.9533333333333296</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43859</v>
       </c>
@@ -628,7 +707,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43860</v>
       </c>
@@ -642,7 +721,7 @@
         <v>4.8061538461538396</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43861</v>
       </c>
@@ -656,7 +735,7 @@
         <v>4.03615384615384</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43862</v>
       </c>
@@ -670,7 +749,7 @@
         <v>4.03615384615384</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43863</v>
       </c>
@@ -684,7 +763,7 @@
         <v>3.76948717948718</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43864</v>
       </c>
@@ -698,7 +777,7 @@
         <v>3.3961538461538399</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43865</v>
       </c>
@@ -712,7 +791,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43866</v>
       </c>
@@ -726,7 +805,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43867</v>
       </c>
@@ -740,7 +819,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43868</v>
       </c>
@@ -754,7 +833,7 @@
         <v>2.5406060606060601</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43869</v>
       </c>
@@ -768,7 +847,7 @@
         <v>2.4239393939393898</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43870</v>
       </c>
@@ -782,7 +861,7 @@
         <v>2.5483838383838302</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43871</v>
       </c>
@@ -796,7 +875,7 @@
         <v>2.5271072426391501</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43872</v>
       </c>
@@ -810,7 +889,7 @@
         <v>2.6951072426391498</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43873</v>
       </c>
@@ -824,7 +903,7 @@
         <v>2.5356506073204499</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43874</v>
       </c>
@@ -838,7 +917,7 @@
         <v>2.3946058312010399</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43875</v>
       </c>
@@ -852,7 +931,7 @@
         <v>2.3868280534232702</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43876</v>
       </c>
@@ -866,7 +945,7 @@
         <v>2.2827713158346099</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43877</v>
       </c>
@@ -880,7 +959,7 @@
         <v>1.9802258612891599</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43878</v>
       </c>
@@ -894,7 +973,7 @@
         <v>1.6494468063721801</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43879</v>
       </c>
@@ -908,7 +987,7 @@
         <v>1.44049158249158</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43880</v>
       </c>
@@ -922,7 +1001,7 @@
         <v>1.3571582491582499</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43881</v>
       </c>
@@ -936,7 +1015,7 @@
         <v>1.2824915824915799</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43882</v>
       </c>
@@ -950,7 +1029,7 @@
         <v>1.2688017429193901</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43883</v>
       </c>
@@ -964,7 +1043,7 @@
         <v>1.16509803921568</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43884</v>
       </c>
@@ -978,7 +1057,7 @@
         <v>1.2280193875302901</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43885</v>
       </c>
@@ -992,7 +1071,7 @@
         <v>1.2562245157354199</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43886</v>
       </c>
@@ -1006,7 +1085,7 @@
         <v>1.2562245157354199</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43887</v>
       </c>
@@ -1023,7 +1102,7 @@
         <v>1.12445980985306</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43888</v>
       </c>
@@ -1049,7 +1128,7 @@
         <v>1.8484196294002799</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43889</v>
       </c>
@@ -1078,7 +1157,7 @@
         <v>2.0954784527240999</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43890</v>
       </c>
@@ -1113,7 +1192,7 @@
         <v>2.6741747961263198</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43891</v>
       </c>
@@ -1154,7 +1233,7 @@
         <v>3.1964805605373501</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43892</v>
       </c>
@@ -1201,7 +1280,7 @@
         <v>3.8355220567383999</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43893</v>
       </c>
@@ -1248,7 +1327,7 @@
         <v>4.7400410723983599</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43894</v>
       </c>
@@ -1298,7 +1377,7 @@
         <v>5.0736274101592702</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43895</v>
       </c>
@@ -1351,7 +1430,7 @@
         <v>5.6617025081580303</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43896</v>
       </c>
@@ -1404,7 +1483,7 @@
         <v>5.8982341357344303</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43897</v>
       </c>
@@ -1457,7 +1536,7 @@
         <v>5.5139922667467998</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43898</v>
       </c>
@@ -1513,7 +1592,7 @@
         <v>6.0419718216986302</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43899</v>
       </c>
@@ -1569,7 +1648,7 @@
         <v>6.4014726458097604</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43900</v>
       </c>
@@ -1628,7 +1707,7 @@
         <v>5.7402621172985198</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43901</v>
       </c>
@@ -1687,7 +1766,7 @@
         <v>5.8010932592436397</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43902</v>
       </c>
@@ -1749,7 +1828,7 @@
         <v>6.15391813551964</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43903</v>
       </c>
@@ -1811,7 +1890,7 @@
         <v>5.1407521648345202</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43904</v>
       </c>
@@ -1876,7 +1955,7 @@
         <v>5.1072652248746104</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43905</v>
       </c>
@@ -1944,7 +2023,7 @@
         <v>5.3537260533238902</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43906</v>
       </c>
@@ -2012,7 +2091,7 @@
         <v>5.0788608920965901</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43907</v>
       </c>
@@ -2083,7 +2162,7 @@
         <v>6.5202840477404704</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43908</v>
       </c>
@@ -2157,7 +2236,7 @@
         <v>6.85315823232437</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43909</v>
       </c>
@@ -2231,7 +2310,7 @@
         <v>6.8656918398169697</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43910</v>
       </c>
@@ -2305,7 +2384,7 @@
         <v>6.6238208337720597</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43911</v>
       </c>
@@ -2382,7 +2461,7 @@
         <v>6.9190520046923796</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43912</v>
       </c>
@@ -2462,7 +2541,7 @@
         <v>5.40526157610035</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43913</v>
       </c>
@@ -2542,7 +2621,7 @@
         <v>4.9071890777294298</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43914</v>
       </c>
@@ -2622,7 +2701,7 @@
         <v>4.75667896302995</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43915</v>
       </c>
@@ -2702,7 +2781,7 @@
         <v>4.5123118444889796</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43916</v>
       </c>
@@ -2782,7 +2861,7 @@
         <v>4.16873817229399</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43917</v>
       </c>
@@ -2862,7 +2941,7 @@
         <v>3.98515051593118</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43918</v>
       </c>
@@ -2945,7 +3024,7 @@
         <v>3.7734235517747599</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43919</v>
       </c>
@@ -3028,7 +3107,7 @@
         <v>3.4604930017252902</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43920</v>
       </c>
@@ -3111,7 +3190,7 @@
         <v>3.2383393055329299</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43921</v>
       </c>
@@ -3194,7 +3273,7 @@
         <v>3.0916639096932998</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43922</v>
       </c>
@@ -3277,7 +3356,7 @@
         <v>3.0082947183294899</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43923</v>
       </c>
@@ -3360,7 +3439,7 @@
         <v>2.9309838676009998</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43924</v>
       </c>
@@ -3443,7 +3522,7 @@
         <v>2.73062018331989</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43925</v>
       </c>
@@ -3526,7 +3605,7 @@
         <v>2.6029511502346199</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43926</v>
       </c>
@@ -3609,7 +3688,7 @@
         <v>2.4394979516107602</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43927</v>
       </c>
@@ -3692,7 +3771,7 @@
         <v>2.29697707367907</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43928</v>
       </c>
@@ -3775,7 +3854,7 @@
         <v>2.1814608544068999</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43929</v>
       </c>
@@ -3858,7 +3937,7 @@
         <v>2.1303035025750598</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43930</v>
       </c>
@@ -3941,7 +4020,7 @@
         <v>2.0533193829241001</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43931</v>
       </c>
@@ -4024,7 +4103,7 @@
         <v>1.9716792975336801</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43932</v>
       </c>
@@ -4107,7 +4186,7 @@
         <v>1.87694601777745</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43933</v>
       </c>
@@ -4190,7 +4269,7 @@
         <v>1.7844842433737</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43934</v>
       </c>
@@ -4273,7 +4352,7 @@
         <v>1.71240396518694</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43935</v>
       </c>
@@ -4356,7 +4435,7 @@
         <v>1.6814831783939099</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43936</v>
       </c>
@@ -4439,7 +4518,7 @@
         <v>1.6623600275150701</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43937</v>
       </c>
@@ -4522,7 +4601,7 @@
         <v>1.6647806860657</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43938</v>
       </c>
@@ -4605,7 +4684,7 @@
         <v>1.6360960225196299</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43939</v>
       </c>
@@ -4688,7 +4767,7 @@
         <v>1.5981029034338301</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43940</v>
       </c>
@@ -4771,7 +4850,7 @@
         <v>1.5589478491027999</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43941</v>
       </c>
@@ -4854,7 +4933,7 @@
         <v>1.52249992125095</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43942</v>
       </c>
@@ -4937,7 +5016,7 @@
         <v>1.4885045227850999</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43943</v>
       </c>
@@ -5020,7 +5099,7 @@
         <v>1.50331572027676</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>43944</v>
       </c>
@@ -5103,7 +5182,7 @@
         <v>1.5105863298054301</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>43945</v>
       </c>
@@ -5186,7 +5265,7 @@
         <v>1.4947406960463001</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>43946</v>
       </c>
@@ -5269,7 +5348,7 @@
         <v>1.4614735567291699</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43947</v>
       </c>
@@ -5352,7 +5431,7 @@
         <v>1.4345438580866201</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43948</v>
       </c>
@@ -5435,7 +5514,7 @@
         <v>1.3935303563724499</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43949</v>
       </c>
@@ -5518,7 +5597,7 @@
         <v>1.3715726072438701</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43950</v>
       </c>
@@ -5601,7 +5680,7 @@
         <v>1.3782223077767299</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43951</v>
       </c>
@@ -5684,7 +5763,7 @@
         <v>1.3870301014019599</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43952</v>
       </c>
@@ -5767,7 +5846,7 @@
         <v>1.38098324957394</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43953</v>
       </c>
@@ -5850,7 +5929,7 @@
         <v>1.3594217223780101</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>43954</v>
       </c>
@@ -5933,7 +6012,7 @@
         <v>1.3368254361626499</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43955</v>
       </c>
@@ -6016,7 +6095,7 @@
         <v>1.3040922405818201</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43956</v>
       </c>
@@ -6099,7 +6178,7 @@
         <v>1.29507716477541</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43957</v>
       </c>
@@ -6182,14 +6261,240 @@
         <v>1.2919632199360001</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>43958</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>43959</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{95BF7DF0-1BDC-46AD-8F2F-16B7B9CD3792}">
+  <dimension ref="A3:B28"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:C28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="14.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>6</v>
+      </c>
+      <c r="B9" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>7</v>
+      </c>
+      <c r="B10" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>14</v>
+      </c>
+      <c r="B17" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>16</v>
+      </c>
+      <c r="B19" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B20" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>18</v>
+      </c>
+      <c r="B21" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>19</v>
+      </c>
+      <c r="B22" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B23" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>22</v>
+      </c>
+      <c r="B25" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>23</v>
+      </c>
+      <c r="B26" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>24</v>
+      </c>
+      <c r="B27" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>43</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
agregué header a la primera columna
</commit_message>
<xml_diff>
--- a/SIR_provincias/r0avanzadas.xlsx
+++ b/SIR_provincias/r0avanzadas.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Johan Rosa\Desktop\Proyectos R\covid_rd_seir\SIR_provincias\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D1A06A6A-7259-4CCD-818D-F9D8CA833E7A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DF95BB78-E485-4C0B-9C58-C1B2B8F5A3C1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E304EFAB-3164-4D20-84F7-4CCF7EACFDA5}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{E304EFAB-3164-4D20-84F7-4CCF7EACFDA5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>R0_AUS_VA7D</t>
   </si>
@@ -109,6 +109,9 @@
   </si>
   <si>
     <t>R0_USA_VA7D</t>
+  </si>
+  <si>
+    <t>fecha</t>
   </si>
 </sst>
 </file>
@@ -464,12 +467,18 @@
   <dimension ref="A1:AA109"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>26</v>
+      </c>
       <c r="B1" t="s">
         <v>0</v>
       </c>
@@ -549,22 +558,22 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>43852</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>43853</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>43854</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>43855</v>
       </c>
@@ -575,7 +584,7 @@
         <v>6.1333333335389204</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>43856</v>
       </c>
@@ -586,7 +595,7 @@
         <v>6.1333333333333302</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>43857</v>
       </c>
@@ -600,7 +609,7 @@
         <v>3.7533333385127201</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>43858</v>
       </c>
@@ -614,7 +623,7 @@
         <v>4.9533333333333296</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>43859</v>
       </c>
@@ -628,7 +637,7 @@
         <v>4.8600000000000003</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>43860</v>
       </c>
@@ -642,7 +651,7 @@
         <v>4.8061538461538396</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>43861</v>
       </c>
@@ -656,7 +665,7 @@
         <v>4.03615384615384</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>43862</v>
       </c>
@@ -670,7 +679,7 @@
         <v>4.03615384615384</v>
       </c>
     </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>43863</v>
       </c>
@@ -684,7 +693,7 @@
         <v>3.76948717948718</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>43864</v>
       </c>
@@ -698,7 +707,7 @@
         <v>3.3961538461538399</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>43865</v>
       </c>
@@ -712,7 +721,7 @@
         <v>2.75</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>43866</v>
       </c>
@@ -726,7 +735,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="17" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>43867</v>
       </c>
@@ -740,7 +749,7 @@
         <v>2.88</v>
       </c>
     </row>
-    <row r="18" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>43868</v>
       </c>
@@ -754,7 +763,7 @@
         <v>2.5406060606060601</v>
       </c>
     </row>
-    <row r="19" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>43869</v>
       </c>
@@ -768,7 +777,7 @@
         <v>2.4239393939393898</v>
       </c>
     </row>
-    <row r="20" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>43870</v>
       </c>
@@ -782,7 +791,7 @@
         <v>2.5483838383838302</v>
       </c>
     </row>
-    <row r="21" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>43871</v>
       </c>
@@ -796,7 +805,7 @@
         <v>2.5271072426391501</v>
       </c>
     </row>
-    <row r="22" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <v>43872</v>
       </c>
@@ -810,7 +819,7 @@
         <v>2.6951072426391498</v>
       </c>
     </row>
-    <row r="23" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <v>43873</v>
       </c>
@@ -824,7 +833,7 @@
         <v>2.5356506073204499</v>
       </c>
     </row>
-    <row r="24" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <v>43874</v>
       </c>
@@ -838,7 +847,7 @@
         <v>2.3946058312010399</v>
       </c>
     </row>
-    <row r="25" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <v>43875</v>
       </c>
@@ -852,7 +861,7 @@
         <v>2.3868280534232702</v>
       </c>
     </row>
-    <row r="26" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <v>43876</v>
       </c>
@@ -866,7 +875,7 @@
         <v>2.2827713158346099</v>
       </c>
     </row>
-    <row r="27" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <v>43877</v>
       </c>
@@ -880,7 +889,7 @@
         <v>1.9802258612891599</v>
       </c>
     </row>
-    <row r="28" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <v>43878</v>
       </c>
@@ -894,7 +903,7 @@
         <v>1.6494468063721801</v>
       </c>
     </row>
-    <row r="29" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <v>43879</v>
       </c>
@@ -908,7 +917,7 @@
         <v>1.44049158249158</v>
       </c>
     </row>
-    <row r="30" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <v>43880</v>
       </c>
@@ -922,7 +931,7 @@
         <v>1.3571582491582499</v>
       </c>
     </row>
-    <row r="31" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <v>43881</v>
       </c>
@@ -936,7 +945,7 @@
         <v>1.2824915824915799</v>
       </c>
     </row>
-    <row r="32" spans="1:24" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <v>43882</v>
       </c>
@@ -950,7 +959,7 @@
         <v>1.2688017429193901</v>
       </c>
     </row>
-    <row r="33" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <v>43883</v>
       </c>
@@ -964,7 +973,7 @@
         <v>1.16509803921568</v>
       </c>
     </row>
-    <row r="34" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <v>43884</v>
       </c>
@@ -978,7 +987,7 @@
         <v>1.2280193875302901</v>
       </c>
     </row>
-    <row r="35" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A35" s="1">
         <v>43885</v>
       </c>
@@ -992,7 +1001,7 @@
         <v>1.2562245157354199</v>
       </c>
     </row>
-    <row r="36" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A36" s="1">
         <v>43886</v>
       </c>
@@ -1006,7 +1015,7 @@
         <v>1.2562245157354199</v>
       </c>
     </row>
-    <row r="37" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A37" s="1">
         <v>43887</v>
       </c>
@@ -1023,7 +1032,7 @@
         <v>1.12445980985306</v>
       </c>
     </row>
-    <row r="38" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A38" s="1">
         <v>43888</v>
       </c>
@@ -1049,7 +1058,7 @@
         <v>1.8484196294002799</v>
       </c>
     </row>
-    <row r="39" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A39" s="1">
         <v>43889</v>
       </c>
@@ -1078,7 +1087,7 @@
         <v>2.0954784527240999</v>
       </c>
     </row>
-    <row r="40" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A40" s="1">
         <v>43890</v>
       </c>
@@ -1113,7 +1122,7 @@
         <v>2.6741747961263198</v>
       </c>
     </row>
-    <row r="41" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A41" s="1">
         <v>43891</v>
       </c>
@@ -1154,7 +1163,7 @@
         <v>3.1964805605373501</v>
       </c>
     </row>
-    <row r="42" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A42" s="1">
         <v>43892</v>
       </c>
@@ -1201,7 +1210,7 @@
         <v>3.8355220567383999</v>
       </c>
     </row>
-    <row r="43" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A43" s="1">
         <v>43893</v>
       </c>
@@ -1248,7 +1257,7 @@
         <v>4.7400410723983599</v>
       </c>
     </row>
-    <row r="44" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A44" s="1">
         <v>43894</v>
       </c>
@@ -1298,7 +1307,7 @@
         <v>5.0736274101592702</v>
       </c>
     </row>
-    <row r="45" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A45" s="1">
         <v>43895</v>
       </c>
@@ -1351,7 +1360,7 @@
         <v>5.6617025081580303</v>
       </c>
     </row>
-    <row r="46" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A46" s="1">
         <v>43896</v>
       </c>
@@ -1404,7 +1413,7 @@
         <v>5.8982341357344303</v>
       </c>
     </row>
-    <row r="47" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A47" s="1">
         <v>43897</v>
       </c>
@@ -1457,7 +1466,7 @@
         <v>5.5139922667467998</v>
       </c>
     </row>
-    <row r="48" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A48" s="1">
         <v>43898</v>
       </c>
@@ -1513,7 +1522,7 @@
         <v>6.0419718216986302</v>
       </c>
     </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A49" s="1">
         <v>43899</v>
       </c>
@@ -1569,7 +1578,7 @@
         <v>6.4014726458097604</v>
       </c>
     </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A50" s="1">
         <v>43900</v>
       </c>
@@ -1628,7 +1637,7 @@
         <v>5.7402621172985198</v>
       </c>
     </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A51" s="1">
         <v>43901</v>
       </c>
@@ -1687,7 +1696,7 @@
         <v>5.8010932592436397</v>
       </c>
     </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A52" s="1">
         <v>43902</v>
       </c>
@@ -1749,7 +1758,7 @@
         <v>6.15391813551964</v>
       </c>
     </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A53" s="1">
         <v>43903</v>
       </c>
@@ -1811,7 +1820,7 @@
         <v>5.1407521648345202</v>
       </c>
     </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A54" s="1">
         <v>43904</v>
       </c>
@@ -1876,7 +1885,7 @@
         <v>5.1072652248746104</v>
       </c>
     </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A55" s="1">
         <v>43905</v>
       </c>
@@ -1944,7 +1953,7 @@
         <v>5.3537260533238902</v>
       </c>
     </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A56" s="1">
         <v>43906</v>
       </c>
@@ -2012,7 +2021,7 @@
         <v>5.0788608920965901</v>
       </c>
     </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A57" s="1">
         <v>43907</v>
       </c>
@@ -2083,7 +2092,7 @@
         <v>6.5202840477404704</v>
       </c>
     </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A58" s="1">
         <v>43908</v>
       </c>
@@ -2157,7 +2166,7 @@
         <v>6.85315823232437</v>
       </c>
     </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A59" s="1">
         <v>43909</v>
       </c>
@@ -2231,7 +2240,7 @@
         <v>6.8656918398169697</v>
       </c>
     </row>
-    <row r="60" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
         <v>43910</v>
       </c>
@@ -2305,7 +2314,7 @@
         <v>6.6238208337720597</v>
       </c>
     </row>
-    <row r="61" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A61" s="1">
         <v>43911</v>
       </c>
@@ -2382,7 +2391,7 @@
         <v>6.9190520046923796</v>
       </c>
     </row>
-    <row r="62" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A62" s="1">
         <v>43912</v>
       </c>
@@ -2462,7 +2471,7 @@
         <v>5.40526157610035</v>
       </c>
     </row>
-    <row r="63" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A63" s="1">
         <v>43913</v>
       </c>
@@ -2542,7 +2551,7 @@
         <v>4.9071890777294298</v>
       </c>
     </row>
-    <row r="64" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A64" s="1">
         <v>43914</v>
       </c>
@@ -2622,7 +2631,7 @@
         <v>4.75667896302995</v>
       </c>
     </row>
-    <row r="65" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A65" s="1">
         <v>43915</v>
       </c>
@@ -2702,7 +2711,7 @@
         <v>4.5123118444889796</v>
       </c>
     </row>
-    <row r="66" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A66" s="1">
         <v>43916</v>
       </c>
@@ -2782,7 +2791,7 @@
         <v>4.16873817229399</v>
       </c>
     </row>
-    <row r="67" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A67" s="1">
         <v>43917</v>
       </c>
@@ -2862,7 +2871,7 @@
         <v>3.98515051593118</v>
       </c>
     </row>
-    <row r="68" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A68" s="1">
         <v>43918</v>
       </c>
@@ -2945,7 +2954,7 @@
         <v>3.7734235517747599</v>
       </c>
     </row>
-    <row r="69" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A69" s="1">
         <v>43919</v>
       </c>
@@ -3028,7 +3037,7 @@
         <v>3.4604930017252902</v>
       </c>
     </row>
-    <row r="70" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A70" s="1">
         <v>43920</v>
       </c>
@@ -3111,7 +3120,7 @@
         <v>3.2383393055329299</v>
       </c>
     </row>
-    <row r="71" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A71" s="1">
         <v>43921</v>
       </c>
@@ -3194,7 +3203,7 @@
         <v>3.0916639096932998</v>
       </c>
     </row>
-    <row r="72" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A72" s="1">
         <v>43922</v>
       </c>
@@ -3277,7 +3286,7 @@
         <v>3.0082947183294899</v>
       </c>
     </row>
-    <row r="73" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A73" s="1">
         <v>43923</v>
       </c>
@@ -3360,7 +3369,7 @@
         <v>2.9309838676009998</v>
       </c>
     </row>
-    <row r="74" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A74" s="1">
         <v>43924</v>
       </c>
@@ -3443,7 +3452,7 @@
         <v>2.73062018331989</v>
       </c>
     </row>
-    <row r="75" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A75" s="1">
         <v>43925</v>
       </c>
@@ -3526,7 +3535,7 @@
         <v>2.6029511502346199</v>
       </c>
     </row>
-    <row r="76" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A76" s="1">
         <v>43926</v>
       </c>
@@ -3609,7 +3618,7 @@
         <v>2.4394979516107602</v>
       </c>
     </row>
-    <row r="77" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A77" s="1">
         <v>43927</v>
       </c>
@@ -3692,7 +3701,7 @@
         <v>2.29697707367907</v>
       </c>
     </row>
-    <row r="78" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A78" s="1">
         <v>43928</v>
       </c>
@@ -3775,7 +3784,7 @@
         <v>2.1814608544068999</v>
       </c>
     </row>
-    <row r="79" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A79" s="1">
         <v>43929</v>
       </c>
@@ -3858,7 +3867,7 @@
         <v>2.1303035025750598</v>
       </c>
     </row>
-    <row r="80" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A80" s="1">
         <v>43930</v>
       </c>
@@ -3941,7 +3950,7 @@
         <v>2.0533193829241001</v>
       </c>
     </row>
-    <row r="81" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A81" s="1">
         <v>43931</v>
       </c>
@@ -4024,7 +4033,7 @@
         <v>1.9716792975336801</v>
       </c>
     </row>
-    <row r="82" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A82" s="1">
         <v>43932</v>
       </c>
@@ -4107,7 +4116,7 @@
         <v>1.87694601777745</v>
       </c>
     </row>
-    <row r="83" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A83" s="1">
         <v>43933</v>
       </c>
@@ -4190,7 +4199,7 @@
         <v>1.7844842433737</v>
       </c>
     </row>
-    <row r="84" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A84" s="1">
         <v>43934</v>
       </c>
@@ -4273,7 +4282,7 @@
         <v>1.71240396518694</v>
       </c>
     </row>
-    <row r="85" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A85" s="1">
         <v>43935</v>
       </c>
@@ -4356,7 +4365,7 @@
         <v>1.6814831783939099</v>
       </c>
     </row>
-    <row r="86" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A86" s="1">
         <v>43936</v>
       </c>
@@ -4439,7 +4448,7 @@
         <v>1.6623600275150701</v>
       </c>
     </row>
-    <row r="87" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A87" s="1">
         <v>43937</v>
       </c>
@@ -4522,7 +4531,7 @@
         <v>1.6647806860657</v>
       </c>
     </row>
-    <row r="88" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A88" s="1">
         <v>43938</v>
       </c>
@@ -4605,7 +4614,7 @@
         <v>1.6360960225196299</v>
       </c>
     </row>
-    <row r="89" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A89" s="1">
         <v>43939</v>
       </c>
@@ -4688,7 +4697,7 @@
         <v>1.5981029034338301</v>
       </c>
     </row>
-    <row r="90" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A90" s="1">
         <v>43940</v>
       </c>
@@ -4771,7 +4780,7 @@
         <v>1.5589478491027999</v>
       </c>
     </row>
-    <row r="91" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A91" s="1">
         <v>43941</v>
       </c>
@@ -4854,7 +4863,7 @@
         <v>1.52249992125095</v>
       </c>
     </row>
-    <row r="92" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A92" s="1">
         <v>43942</v>
       </c>
@@ -4937,7 +4946,7 @@
         <v>1.4885045227850999</v>
       </c>
     </row>
-    <row r="93" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A93" s="1">
         <v>43943</v>
       </c>
@@ -5020,7 +5029,7 @@
         <v>1.50331572027676</v>
       </c>
     </row>
-    <row r="94" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A94" s="1">
         <v>43944</v>
       </c>
@@ -5103,7 +5112,7 @@
         <v>1.5105863298054301</v>
       </c>
     </row>
-    <row r="95" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A95" s="1">
         <v>43945</v>
       </c>
@@ -5186,7 +5195,7 @@
         <v>1.4947406960463001</v>
       </c>
     </row>
-    <row r="96" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A96" s="1">
         <v>43946</v>
       </c>
@@ -5269,7 +5278,7 @@
         <v>1.4614735567291699</v>
       </c>
     </row>
-    <row r="97" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A97" s="1">
         <v>43947</v>
       </c>
@@ -5352,7 +5361,7 @@
         <v>1.4345438580866201</v>
       </c>
     </row>
-    <row r="98" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A98" s="1">
         <v>43948</v>
       </c>
@@ -5435,7 +5444,7 @@
         <v>1.3935303563724499</v>
       </c>
     </row>
-    <row r="99" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A99" s="1">
         <v>43949</v>
       </c>
@@ -5518,7 +5527,7 @@
         <v>1.3715726072438701</v>
       </c>
     </row>
-    <row r="100" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A100" s="1">
         <v>43950</v>
       </c>
@@ -5601,7 +5610,7 @@
         <v>1.3782223077767299</v>
       </c>
     </row>
-    <row r="101" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A101" s="1">
         <v>43951</v>
       </c>
@@ -5684,7 +5693,7 @@
         <v>1.3870301014019599</v>
       </c>
     </row>
-    <row r="102" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A102" s="1">
         <v>43952</v>
       </c>
@@ -5767,7 +5776,7 @@
         <v>1.38098324957394</v>
       </c>
     </row>
-    <row r="103" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A103" s="1">
         <v>43953</v>
       </c>
@@ -5850,7 +5859,7 @@
         <v>1.3594217223780101</v>
       </c>
     </row>
-    <row r="104" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A104" s="1">
         <v>43954</v>
       </c>
@@ -5933,7 +5942,7 @@
         <v>1.3368254361626499</v>
       </c>
     </row>
-    <row r="105" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A105" s="1">
         <v>43955</v>
       </c>
@@ -6016,7 +6025,7 @@
         <v>1.3040922405818201</v>
       </c>
     </row>
-    <row r="106" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
         <v>43956</v>
       </c>
@@ -6099,7 +6108,7 @@
         <v>1.29507716477541</v>
       </c>
     </row>
-    <row r="107" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A107" s="1">
         <v>43957</v>
       </c>
@@ -6182,12 +6191,12 @@
         <v>1.2919632199360001</v>
       </c>
     </row>
-    <row r="108" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A108" s="1">
         <v>43958</v>
       </c>
     </row>
-    <row r="109" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:27" x14ac:dyDescent="0.25">
       <c r="A109" s="1">
         <v>43959</v>
       </c>

</xml_diff>